<commit_message>
Tidying/commenting PMS1003 code for hand over
</commit_message>
<xml_diff>
--- a/Testing/Wind tunnel/6th Sept/Wind tunnel OPCN2 Test #2 6th Sept.xlsx
+++ b/Testing/Wind tunnel/6th Sept/Wind tunnel OPCN2 Test #2 6th Sept.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\Testing\Wind tunnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\Testing\Wind tunnel\6th Sept\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Ash Conc Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Flow Rate Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Graph for oral" sheetId="3" r:id="rId2"/>
+    <sheet name="Flow Rate Analysis" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -43,10 +44,10 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Total Conc</t>
+    <t>Injected Ash Conc</t>
   </si>
   <si>
-    <t>Injected Ash Conc</t>
+    <t>OPCN2</t>
   </si>
 </sst>
 </file>
@@ -9607,7 +9608,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total Conc</c:v>
+                  <c:v>OPCN2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11770,6 +11771,2254 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Total Concentration of Ash</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ash Conc Analysis'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OPCN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$A$2:$A$278</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="277"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>78.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>83.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>87.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>91.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>103.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>112.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>116.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>120.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>124.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>128.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>132.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>137.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>141.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>145.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>153.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>157.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>166.1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>170.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>174.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>178.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>182.7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>186.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>195.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>199.3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>203.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>207.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>211.8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>215.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>220.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>224.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>228.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>232.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>236.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>240.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>249.2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>253.3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>257.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>261.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>265.8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>269.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>274.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>278.2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>282.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>286.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>290.7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>294.8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>303.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>307.3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>311.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>315.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>319.7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>323.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>332.2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>336.3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>340.5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>344.6</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>348.8</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>352.9</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>357.1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>361.2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>365.4</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>369.6</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>373.7</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>377.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>386.2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>390.3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>394.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>398.6</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>402.8</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>406.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>411.1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>415.2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>419.4</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>423.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>427.7</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>431.8</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>440.1</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>444.3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>448.4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>452.6</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>456.7</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>460.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>469.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>473.3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>477.5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>481.6</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>485.8</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>489.9</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>494.1</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>498.2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>502.4</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>506.6</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>510.7</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>514.9</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>523.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>527.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>531.5</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>535.6</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>539.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>543.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>548.1</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>552.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>556.4</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>560.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>564.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>568.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>577.1</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>581.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>585.4</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>589.6</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>593.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>597.9</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>606.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>610.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>614.5</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>618.6</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>622.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>626.9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>631.1</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>635.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>639.4</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>643.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>647.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>651.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>656</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>660.1</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>664.3</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>668.4</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>672.6</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>676.8</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>680.9</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>685.1</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>689.2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>693.4</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>697.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>701.7</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>705.8</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>714.1</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>718.3</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>722.4</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>726.6</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>730.7</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>734.9</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>743.2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>747.3</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>751.5</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>755.6</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>759.8</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>763.9</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>768.1</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>772.2</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>776.4</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>780.5</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>784.7</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>788.8</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>797.1</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>801.3</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>805.4</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>809.6</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>813.7</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>817.9</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>822</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>826.2</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>830.3</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>834.5</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>838.7</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>842.8</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>851.1</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>855.3</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>859.4</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>863.6</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>867.7</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>871.9</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>880.2</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>884.3</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>888.5</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>892.6</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>896.8</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>900.9</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>905.1</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>909.2</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>913.4</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>917.5</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>921.7</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>925.8</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>934.1</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>938.3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>942.4</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>946.6</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>950.7</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>954.9</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>963.2</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>967.3</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>971.5</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>975.6</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>979.8</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>983.9</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>988.1</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>992.3</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>996.4</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1000.6</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1004.7</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1008.9</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1017.2</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1021.3</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1025.5</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1029.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1033.8</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1037.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1042.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1046.2</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1050.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1054.5</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1058.7</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1062.8</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1067</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1071.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1075.3</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1079.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1083.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1087.7</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1091.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1100.2</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1104.3</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1108.5</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1112.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1116.8</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1120.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1125.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1129.2</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1133.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1137.5</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1141.7</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1145.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1154.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$G$2:$G$278</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="277"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.71</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10.57</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.93</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.08</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.23</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.84</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.02</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9.24</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.77</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>11.34</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>7.45</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>9.85</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>7.22</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>6.91</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>7.73</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>8.5299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>8.76</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>9.09</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8.74</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>10.92</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7.96</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>8.14</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>7.02</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>7.07</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>6.47</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>7.38</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>8.15</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>7.96</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>6.39</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>8.84</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>6.11</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>9.0299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>8.82</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>8.3699999999999992</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>9.31</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>24.64</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>17.21</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>13.25</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>11.21</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>6.42</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>9.01</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>6.62</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>13.79</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>6.05</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>6.41</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>7.19</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>6.63</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>6.28</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>9.3699999999999992</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5.79</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5.66</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>6.33</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>17.829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>20.96</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>18.34</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>16.440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>18.39</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>20.12</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>23.24</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>20.61</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>28.92</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>22.18</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>24.88</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>24.78</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>17.579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>19.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>25.14</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>15.67</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>20.46</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>21.02</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>24.19</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>15.83</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>21.77</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>19.11</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>19.29</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>10.69</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>16.25</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>19.45</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>17.61</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>17.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>11.42</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>8.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DED-421D-AD3F-828BB28EDA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ash Conc Analysis'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Injected Ash Conc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$J$2:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>805</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$K$2:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DED-421D-AD3F-828BB28EDA5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="303286584"/>
+        <c:axId val="303289208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="303286584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="800"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="303289208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="303289208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Concentration (mg/m^3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="303286584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -13908,6 +16157,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -15484,6 +17773,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15736,6 +18541,43 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16141,7 +18983,7 @@
   <dimension ref="A1:K278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16174,7 +19016,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -16183,7 +19025,7 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -23479,6 +26321,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated testing docs and added OPCN2 Code
</commit_message>
<xml_diff>
--- a/Testing/Wind tunnel/6th Sept/Wind tunnel OPCN2 Test #2 6th Sept.xlsx
+++ b/Testing/Wind tunnel/6th Sept/Wind tunnel OPCN2 Test #2 6th Sept.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Ash Conc Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Only first two injections" sheetId="3" r:id="rId2"/>
-    <sheet name="Flow Rate Analysis" sheetId="2" r:id="rId3"/>
+    <sheet name="Flow Rate Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="For oral and report" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -11790,6 +11790,2064 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ash Conc Analysis'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Flow rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$A$2:$A$278</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="277"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>78.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>83.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>87.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>91.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>103.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>112.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>116.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>120.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>124.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>128.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>132.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>137.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>141.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>145.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>153.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>157.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>166.1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>170.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>174.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>178.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>182.7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>186.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>195.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>199.3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>203.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>207.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>211.8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>215.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>220.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>224.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>228.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>232.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>236.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>240.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>249.2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>253.3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>257.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>261.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>265.8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>269.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>274.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>278.2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>282.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>286.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>290.7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>294.8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>303.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>307.3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>311.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>315.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>319.7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>323.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>332.2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>336.3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>340.5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>344.6</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>348.8</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>352.9</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>357.1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>361.2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>365.4</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>369.6</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>373.7</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>377.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>386.2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>390.3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>394.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>398.6</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>402.8</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>406.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>411.1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>415.2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>419.4</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>423.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>427.7</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>431.8</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>440.1</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>444.3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>448.4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>452.6</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>456.7</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>460.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>469.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>473.3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>477.5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>481.6</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>485.8</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>489.9</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>494.1</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>498.2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>502.4</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>506.6</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>510.7</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>514.9</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>523.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>527.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>531.5</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>535.6</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>539.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>543.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>548.1</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>552.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>556.4</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>560.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>564.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>568.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>577.1</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>581.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>585.4</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>589.6</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>593.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>597.9</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>606.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>610.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>614.5</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>618.6</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>622.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>626.9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>631.1</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>635.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>639.4</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>643.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>647.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>651.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>656</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>660.1</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>664.3</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>668.4</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>672.6</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>676.8</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>680.9</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>685.1</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>689.2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>693.4</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>697.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>701.7</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>705.8</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>714.1</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>718.3</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>722.4</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>726.6</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>730.7</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>734.9</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>743.2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>747.3</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>751.5</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>755.6</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>759.8</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>763.9</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>768.1</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>772.2</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>776.4</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>780.5</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>784.7</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>788.8</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>797.1</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>801.3</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>805.4</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>809.6</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>813.7</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>817.9</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>822</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>826.2</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>830.3</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>834.5</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>838.7</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>842.8</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>851.1</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>855.3</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>859.4</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>863.6</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>867.7</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>871.9</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>880.2</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>884.3</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>888.5</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>892.6</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>896.8</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>900.9</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>905.1</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>909.2</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>913.4</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>917.5</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>921.7</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>925.8</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>934.1</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>938.3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>942.4</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>946.6</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>950.7</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>954.9</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>963.2</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>967.3</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>971.5</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>975.6</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>979.8</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>983.9</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>988.1</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>992.3</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>996.4</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1000.6</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1004.7</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1008.9</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1017.2</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1021.3</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1025.5</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1029.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1033.8</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1037.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1042.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1046.2</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1050.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1054.5</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1058.7</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1062.8</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1067</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1071.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1075.3</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1079.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1083.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1087.7</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1091.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1100.2</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1104.3</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1108.5</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1112.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1116.8</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1120.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1125.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1129.2</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1133.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1137.5</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1141.7</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1145.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1154.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$H$2:$H$278</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="277"/>
+                <c:pt idx="0">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-384D-4E15-9280-1F41D9B24239}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="501496944"/>
+        <c:axId val="501495960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="501496944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501495960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="501495960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>FLow Rate (mL/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501496944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -14023,7 +16081,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14037,37 +16095,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -14078,11 +16106,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ash Conc Analysis'!$H$1</c:f>
+              <c:f>'Ash Conc Analysis'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Flow rate</c:v>
+                  <c:v>OPCN2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14941,840 +16969,840 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ash Conc Analysis'!$H$2:$H$278</c:f>
+              <c:f>'Ash Conc Analysis'!$G$2:$G$278</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="277"/>
                 <c:pt idx="0">
-                  <c:v>1.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.03</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.03</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.03</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.04</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.05</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.06</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.05</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.07</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.08</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>1.76</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>2.0099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>2.65</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>2.13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>3.24</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.31</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.71</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>10.57</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>9.93</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>11.08</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>8.23</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>9.84</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>9.24</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>8.1199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>6.16</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.77</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>11.34</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>8.59</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.27</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.34</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.31</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.27</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.21</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.1299999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.19</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.22</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.22</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.22</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.22</c:v>
+                  <c:v>9.25</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.22</c:v>
+                  <c:v>7.45</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.22</c:v>
+                  <c:v>5.93</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.22</c:v>
+                  <c:v>9.85</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1.22</c:v>
+                  <c:v>7.22</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.22</c:v>
+                  <c:v>6.91</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.22</c:v>
+                  <c:v>7.73</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.22</c:v>
+                  <c:v>8.5299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.22</c:v>
+                  <c:v>8.76</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.22</c:v>
+                  <c:v>9.09</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1.22</c:v>
+                  <c:v>8.74</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1.22</c:v>
+                  <c:v>10.92</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1.22</c:v>
+                  <c:v>7.96</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1.22</c:v>
+                  <c:v>13.15</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1.22</c:v>
+                  <c:v>8.14</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1.22</c:v>
+                  <c:v>7.02</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1.22</c:v>
+                  <c:v>7.07</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1.22</c:v>
+                  <c:v>6.47</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1.22</c:v>
+                  <c:v>7.38</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1.22</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.22</c:v>
+                  <c:v>8.15</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1.22</c:v>
+                  <c:v>7.96</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1.22</c:v>
+                  <c:v>7.05</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1.22</c:v>
+                  <c:v>6.39</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1.22</c:v>
+                  <c:v>8.84</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1.22</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>1.22</c:v>
+                  <c:v>6.11</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1.22</c:v>
+                  <c:v>9.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1.22</c:v>
+                  <c:v>5.69</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1.22</c:v>
+                  <c:v>8.82</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1.22</c:v>
+                  <c:v>8.3699999999999992</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1.22</c:v>
+                  <c:v>9.31</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1.22</c:v>
+                  <c:v>24.64</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.22</c:v>
+                  <c:v>17.21</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1.22</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>1.22</c:v>
+                  <c:v>11.21</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>1.22</c:v>
+                  <c:v>8.08</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1.22</c:v>
+                  <c:v>5.55</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>1.22</c:v>
+                  <c:v>6.42</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>1.22</c:v>
+                  <c:v>9.01</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>1.22</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>1.22</c:v>
+                  <c:v>6.62</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>1.22</c:v>
+                  <c:v>13.79</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>1.22</c:v>
+                  <c:v>6.05</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>1.22</c:v>
+                  <c:v>6.41</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>1.22</c:v>
+                  <c:v>7.19</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>1.22</c:v>
+                  <c:v>3.69</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>1.22</c:v>
+                  <c:v>6.63</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>1.22</c:v>
+                  <c:v>6.28</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>1.22</c:v>
+                  <c:v>9.3699999999999992</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>1.22</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>1.22</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>1.22</c:v>
+                  <c:v>5.93</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>1.22</c:v>
+                  <c:v>11.17</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>1.22</c:v>
+                  <c:v>5.77</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>1.22</c:v>
+                  <c:v>5.79</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>1.22</c:v>
+                  <c:v>5.66</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>1.22</c:v>
+                  <c:v>6.33</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>1.22</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>1.22</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>1.18</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>1.06</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>1.05</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>1.06</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>1.04</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>1.06</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>1.06</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>1.08</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>1.19</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>1.19</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>1.19</c:v>
+                  <c:v>22.89</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>1.19</c:v>
+                  <c:v>17.829999999999998</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>1.19</c:v>
+                  <c:v>14.95</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>1.19</c:v>
+                  <c:v>20.96</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>1.19</c:v>
+                  <c:v>18.34</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>1.19</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>1.19</c:v>
+                  <c:v>16.440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>1.19</c:v>
+                  <c:v>18.39</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>1.19</c:v>
+                  <c:v>20.12</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>1.19</c:v>
+                  <c:v>23.24</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>1.19</c:v>
+                  <c:v>20.61</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>1.19</c:v>
+                  <c:v>28.92</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>1.19</c:v>
+                  <c:v>22.18</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>1.19</c:v>
+                  <c:v>24.88</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>1.19</c:v>
+                  <c:v>24.78</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>1.19</c:v>
+                  <c:v>17.579999999999998</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>1.19</c:v>
+                  <c:v>19.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>1.19</c:v>
+                  <c:v>25.14</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>1.19</c:v>
+                  <c:v>15.67</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>1.19</c:v>
+                  <c:v>20.46</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>1.19</c:v>
+                  <c:v>21.02</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>1.19</c:v>
+                  <c:v>24.19</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>1.19</c:v>
+                  <c:v>15.83</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>1.19</c:v>
+                  <c:v>21.77</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>1.19</c:v>
+                  <c:v>19.11</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>1.19</c:v>
+                  <c:v>19.29</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>1.19</c:v>
+                  <c:v>10.69</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>1.19</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>1.19</c:v>
+                  <c:v>19.45</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>1.19</c:v>
+                  <c:v>17.61</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>1.19</c:v>
+                  <c:v>17.170000000000002</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>1.19</c:v>
+                  <c:v>11.42</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>1.19</c:v>
+                  <c:v>8.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>1.19</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>1.19</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>1.19</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>1.19</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>1.19</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>1.19</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>1.19</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>1.19</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>1.19</c:v>
+                  <c:v>1.68</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>1.19</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>1.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>1.19</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>1.19</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>1.19</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>1.19</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>1.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>1.19</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>1.19</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>1.19</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>1.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>1.19</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>1.19</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>1.19</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>1.19</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>1.19</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>1.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>1.19</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>1.32</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>1.25</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>1.24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>1.22</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>1.1299999999999999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>1.05</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>1.05</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>1.04</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>1.07</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>1.07</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>1.05</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>1.19</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15782,7 +17810,144 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-384D-4E15-9280-1F41D9B24239}"/>
+              <c16:uniqueId val="{00000000-6C2E-4E12-9C7F-5865A97C19C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ash Conc Analysis'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Injected Ash Conc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$J$2:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>805</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ash Conc Analysis'!$K$2:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6C2E-4E12-9C7F-5865A97C19C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15794,13 +17959,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="501496944"/>
-        <c:axId val="501495960"/>
+        <c:axId val="303286584"/>
+        <c:axId val="303289208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="501496944"/>
+        <c:axId val="303286584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -15825,7 +17991,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15839,13 +18005,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-NZ"/>
-                  <a:t>Time</a:t>
+                  <a:t>Time (s)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" baseline="0"/>
-                  <a:t> (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -15862,7 +18023,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -15900,7 +18061,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15915,12 +18076,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501495960"/>
+        <c:crossAx val="303289208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="501495960"/>
+        <c:axId val="303289208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15947,7 +18108,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15961,11 +18122,19 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-NZ"/>
-                  <a:t>FLow Rate (mL/s)</a:t>
+                  <a:t>Concentration (mg/m^3)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.77000777000777E-3"/>
+              <c:y val="0.19102860745758732"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15979,7 +18148,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -16017,7 +18186,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -16032,7 +18201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501496944"/>
+        <c:crossAx val="303286584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16044,6 +18213,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -16068,7 +18268,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1600"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -16202,6 +18402,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -18294,6 +20534,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -18843,43 +21599,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -18977,6 +21696,75 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -26624,7 +29412,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26639,7 +29427,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>